<commit_message>
역할 분담 _2025.08.08 JHE
역할 분담 업데이트
</commit_message>
<xml_diff>
--- a/자바 쇼핑몰 프젝 가이드.xlsx
+++ b/자바 쇼핑몰 프젝 가이드.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\자바 교육\6. 쇼핑몰 프로젝트(2025.08.07~21)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557BD278-A299-4152-97B5-41A894FD7EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036DAD3B-371A-461B-A358-1BB7BFC7586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{8BC8CA94-ABF4-4AEF-B910-733F5AB02897}"/>
   </bookViews>
@@ -19,7 +19,11 @@
     <sheet name="GitHub" sheetId="5" r:id="rId4"/>
     <sheet name="깃허브 업로드" sheetId="4" state="hidden" r:id="rId5"/>
     <sheet name="역할 분담" sheetId="6" r:id="rId6"/>
+    <sheet name="report" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'역할 분담'!$B$2:$I$69</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="500">
   <si>
     <t>논의 시간 : (8/8 금) 오전에 논의 시간 줌</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2848,6 +2852,45 @@
 3) checkNotNull(Object obj, String message)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14일 까지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User extends Role</t>
+  </si>
+  <si>
+    <t>Role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Admin extends Role</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>FrontController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2856,7 +2899,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2994,8 +3037,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3016,6 +3067,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -3160,7 +3217,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3170,8 +3227,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3281,25 +3341,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3315,9 +3357,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
@@ -3338,7 +3377,22 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -3350,8 +3404,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="20% - 강조색1" xfId="3" builtinId="30"/>
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
     <cellStyle name="보통" xfId="2" builtinId="28"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3709,7 +3767,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X9" sqref="X9"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4279,7 +4337,7 @@
   <dimension ref="B2:C400"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G270" sqref="G270"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4323,7 +4381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:3" s="19" customFormat="1"/>
+    <row r="14" spans="2:3" s="54" customFormat="1"/>
     <row r="16" spans="2:3">
       <c r="B16" s="16" t="s">
         <v>28</v>
@@ -6120,7 +6178,7 @@
   <dimension ref="B3:U32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC23" sqref="AC23"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6385,25 +6443,25 @@
   <sheetData>
     <row r="1" spans="2:15" ht="17.25" thickBot="1"/>
     <row r="2" spans="2:15">
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="35" t="s">
         <v>382</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="36" t="s">
         <v>383</v>
       </c>
-      <c r="O2" s="43"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="2:15">
       <c r="B3" t="s">
         <v>299</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="38" t="s">
         <v>379</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" t="s">
         <v>384</v>
       </c>
-      <c r="O3" s="46"/>
+      <c r="O3" s="39"/>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -6412,22 +6470,22 @@
       <c r="H4" t="s">
         <v>326</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="38" t="s">
         <v>380</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" t="s">
         <v>385</v>
       </c>
-      <c r="O4" s="46"/>
+      <c r="O4" s="39"/>
     </row>
     <row r="5" spans="2:15" ht="17.25" thickBot="1">
-      <c r="M5" s="47" t="s">
+      <c r="M5" s="40" t="s">
         <v>381</v>
       </c>
-      <c r="N5" s="48" t="s">
+      <c r="N5" s="41" t="s">
         <v>386</v>
       </c>
-      <c r="O5" s="49"/>
+      <c r="O5" s="42"/>
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
@@ -6568,959 +6626,1156 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C388FA55-A5F7-46B9-B73C-9EEEF04696AA}">
-  <dimension ref="B2:H69"/>
+  <dimension ref="B2:J71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="4.125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" style="50" customWidth="1"/>
-    <col min="4" max="4" width="17.75" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.25" style="50" customWidth="1"/>
-    <col min="6" max="6" width="95" style="50" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.25" style="50" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="50"/>
+    <col min="1" max="1" width="4.125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="12.125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="17.75" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.25" style="43" customWidth="1"/>
+    <col min="6" max="6" width="95" style="43" customWidth="1"/>
+    <col min="7" max="7" width="7.125" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.25" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="43"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="B2" s="40" t="s">
+    <row r="2" spans="2:9">
+      <c r="B2" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="34" t="s">
         <v>411</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="34" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="181.5">
-      <c r="B3" s="33" t="s">
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="2:9" ht="181.5">
+      <c r="B3" s="45" t="s">
         <v>364</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="34" t="s">
         <v>476</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="34" t="s">
         <v>474</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="52"/>
-    </row>
-    <row r="4" spans="2:8" ht="165">
-      <c r="B4" s="38"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+    </row>
+    <row r="4" spans="2:9" ht="165">
+      <c r="B4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="34" t="s">
         <v>439</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="34" t="s">
         <v>475</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="52"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="39"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="52"/>
-    </row>
-    <row r="6" spans="2:8" ht="165">
-      <c r="B6" s="53" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="46"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="2:9" ht="165">
+      <c r="B6" s="51" t="s">
         <v>365</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="45" t="s">
         <v>351</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>340</v>
-      </c>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="34" t="s">
+        <v>491</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>416</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="34" t="s">
         <v>387</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="34" t="s">
         <v>341</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" ht="247.5">
-      <c r="B7" s="54"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="40" t="s">
+    <row r="7" spans="2:9" ht="247.5">
+      <c r="B7" s="52"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="34" t="s">
         <v>406</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="34" t="s">
         <v>413</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="34" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="264">
-      <c r="B8" s="54"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="40" t="s">
+    <row r="8" spans="2:9" ht="264">
+      <c r="B8" s="52"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="34" t="s">
         <v>392</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="34" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="165">
-      <c r="B9" s="54"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="40" t="s">
-        <v>343</v>
-      </c>
-      <c r="E9" s="40" t="s">
+    <row r="9" spans="2:9" ht="165">
+      <c r="B9" s="52"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="34" t="s">
+        <v>494</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>417</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="34" t="s">
         <v>388</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="34" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="181.5">
-      <c r="B10" s="54"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="40" t="s">
+    <row r="10" spans="2:9" ht="181.5">
+      <c r="B10" s="52"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="43" t="s">
         <v>418</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="34" t="s">
         <v>389</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="34" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="264">
-      <c r="B11" s="54"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="40" t="s">
+    <row r="11" spans="2:9" ht="264">
+      <c r="B11" s="52"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="34" t="s">
         <v>407</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="34" t="s">
         <v>415</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="34" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="148.5">
-      <c r="B12" s="54"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="40" t="s">
+    <row r="12" spans="2:9" ht="148.5">
+      <c r="B12" s="52"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="34" t="s">
         <v>377</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="44" t="s">
         <v>420</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="34" t="s">
         <v>390</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-    </row>
-    <row r="13" spans="2:8" ht="82.5">
-      <c r="B13" s="54"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="40" t="s">
+      <c r="G12" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="2:9" ht="82.5">
+      <c r="B13" s="52"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="34" t="s">
         <v>391</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="54"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="55"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-    </row>
-    <row r="16" spans="2:8" ht="220.5" customHeight="1">
-      <c r="B16" s="53" t="s">
+      <c r="G13" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="52"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="53"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+    </row>
+    <row r="16" spans="2:9" ht="220.5" customHeight="1">
+      <c r="B16" s="51" t="s">
         <v>366</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="34" t="s">
         <v>430</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="45" t="s">
         <v>470</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="G16" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="54"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="40" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="34" t="s">
         <v>434</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="2:8" ht="191.25" customHeight="1">
-      <c r="B18" s="54"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="40" t="s">
+      <c r="B18" s="52"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="34" t="s">
         <v>431</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="33" t="s">
+      <c r="E18" s="34"/>
+      <c r="F18" s="45" t="s">
         <v>471</v>
       </c>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
+      <c r="G18" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="2:8" ht="33">
-      <c r="B19" s="54"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="40" t="s">
+      <c r="B19" s="52"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="34" t="s">
         <v>435</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="2:8" ht="183.75" customHeight="1">
-      <c r="B20" s="54"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="40" t="s">
+      <c r="B20" s="52"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="34" t="s">
         <v>432</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="33" t="s">
+      <c r="E20" s="34"/>
+      <c r="F20" s="45" t="s">
         <v>472</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
+      <c r="G20" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="54"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="40" t="s">
+      <c r="B21" s="52"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="34" t="s">
         <v>436</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="2:8" ht="265.5" customHeight="1">
-      <c r="B22" s="54"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="40" t="s">
+      <c r="B22" s="52"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="33" t="s">
+      <c r="E22" s="34"/>
+      <c r="F22" s="45" t="s">
         <v>473</v>
       </c>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
+      <c r="G22" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="54"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="40" t="s">
+      <c r="B23" s="52"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="34" t="s">
         <v>437</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="54"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="55"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="2:8" ht="165">
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="51" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="34" t="s">
         <v>409</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="34" t="s">
         <v>426</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
+      <c r="G26" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="2:8" ht="115.5">
-      <c r="B27" s="54"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="40" t="s">
+      <c r="B27" s="52"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="34" t="s">
         <v>403</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="34" t="s">
         <v>427</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="34" t="s">
         <v>463</v>
       </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
+      <c r="G27" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="2:8" ht="99">
-      <c r="B28" s="54"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="40" t="s">
+      <c r="B28" s="52"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="34" t="s">
         <v>404</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="34" t="s">
         <v>464</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
+      <c r="G28" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="2:8" ht="132">
-      <c r="B29" s="54"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="40" t="s">
+      <c r="B29" s="52"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="34" t="s">
         <v>405</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="34" t="s">
         <v>429</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="34" t="s">
         <v>465</v>
       </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
+      <c r="G29" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="2:8" ht="82.5">
-      <c r="B30" s="54"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="40" t="s">
+      <c r="B30" s="52"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="34" t="s">
         <v>466</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40" t="s">
+      <c r="E30" s="34"/>
+      <c r="F30" s="34" t="s">
         <v>468</v>
       </c>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
+      <c r="G30" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="2:8" ht="99">
-      <c r="B31" s="54"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="40" t="s">
+      <c r="B31" s="52"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="34" t="s">
         <v>467</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40" t="s">
+      <c r="E31" s="34"/>
+      <c r="F31" s="34" t="s">
         <v>469</v>
       </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
+      <c r="G31" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="55"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="33" t="s">
+      <c r="B32" s="53"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="45" t="s">
         <v>368</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="40" t="s">
+      <c r="C33" s="45"/>
+      <c r="D33" s="34" t="s">
         <v>452</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="34" t="s">
         <v>455</v>
       </c>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-    </row>
-    <row r="34" spans="2:8" ht="165">
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="40" t="s">
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="2:10" ht="165">
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="34" t="s">
         <v>453</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="34" t="s">
         <v>480</v>
       </c>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="40" t="s">
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="34" t="s">
         <v>456</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="40" t="s">
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-    </row>
-    <row r="37" spans="2:8" ht="33">
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="40" t="s">
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+    </row>
+    <row r="37" spans="2:10" ht="33">
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="34" t="s">
         <v>458</v>
       </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" spans="2:8" ht="33">
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="40" t="s">
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+    </row>
+    <row r="38" spans="2:10" ht="33">
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="34" t="s">
         <v>459</v>
       </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-    </row>
-    <row r="41" spans="2:8" ht="148.5">
-      <c r="B41" s="53" t="s">
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+    </row>
+    <row r="41" spans="2:10" ht="148.5">
+      <c r="B41" s="51" t="s">
         <v>369</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="48" t="s">
         <v>355</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="34" t="s">
         <v>398</v>
       </c>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-    </row>
-    <row r="42" spans="2:8" ht="148.5">
-      <c r="B42" s="54"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="40" t="s">
+      <c r="G41" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="H41" s="34"/>
+    </row>
+    <row r="42" spans="2:10" ht="148.5">
+      <c r="B42" s="52"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="34" t="s">
         <v>408</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" s="34" t="s">
         <v>402</v>
       </c>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-    </row>
-    <row r="43" spans="2:8" ht="165">
-      <c r="B43" s="54"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="40" t="s">
+      <c r="G42" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="H42" s="34"/>
+    </row>
+    <row r="43" spans="2:10" ht="165">
+      <c r="B43" s="52"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="34" t="s">
         <v>395</v>
       </c>
-      <c r="E43" s="40" t="s">
+      <c r="E43" s="34" t="s">
         <v>423</v>
       </c>
-      <c r="F43" s="40" t="s">
+      <c r="F43" s="34" t="s">
         <v>399</v>
       </c>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-    </row>
-    <row r="44" spans="2:8" ht="165">
-      <c r="B44" s="54"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="40" t="s">
+      <c r="G43" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="H43" s="34"/>
+    </row>
+    <row r="44" spans="2:10" ht="165">
+      <c r="B44" s="52"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="34" t="s">
         <v>396</v>
       </c>
-      <c r="E44" s="40" t="s">
+      <c r="E44" s="34" t="s">
         <v>424</v>
       </c>
-      <c r="F44" s="40" t="s">
+      <c r="F44" s="34" t="s">
         <v>400</v>
       </c>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-    </row>
-    <row r="45" spans="2:8" ht="148.5">
-      <c r="B45" s="54"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="40" t="s">
+      <c r="G44" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="H44" s="34"/>
+    </row>
+    <row r="45" spans="2:10" ht="148.5">
+      <c r="B45" s="52"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="E45" s="50" t="s">
+      <c r="E45" s="43" t="s">
         <v>425</v>
       </c>
-      <c r="F45" s="40" t="s">
+      <c r="F45" s="34" t="s">
         <v>401</v>
       </c>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" s="54"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="40" t="s">
+      <c r="G45" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="H45" s="34"/>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="52"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="34" t="s">
         <v>460</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="34" t="s">
         <v>461</v>
       </c>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-    </row>
-    <row r="47" spans="2:8">
-      <c r="B47" s="55"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-    </row>
-    <row r="48" spans="2:8">
-      <c r="B48" s="33" t="s">
+      <c r="F46" s="34"/>
+      <c r="G46" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="H46" s="34"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="53"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="45" t="s">
         <v>356</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="48" t="s">
         <v>359</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="34" t="s">
         <v>372</v>
       </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" s="38"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="40" t="s">
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48"/>
+      <c r="J48"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="47"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-    </row>
-    <row r="50" spans="2:8" ht="165">
-      <c r="B50" s="38"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="40" t="s">
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="2:10" ht="165">
+      <c r="B50" s="47"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="34" t="s">
         <v>482</v>
       </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40" t="s">
+      <c r="E50" s="34"/>
+      <c r="F50" s="34" t="s">
         <v>488</v>
       </c>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-    </row>
-    <row r="51" spans="2:8" ht="198">
-      <c r="B51" s="38"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="40" t="s">
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="2:10" ht="198">
+      <c r="B51" s="47"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E51" s="40" t="s">
+      <c r="E51" s="34" t="s">
         <v>447</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="34" t="s">
         <v>481</v>
       </c>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-    </row>
-    <row r="52" spans="2:8" ht="175.5" customHeight="1">
-      <c r="B52" s="38"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="40" t="s">
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="2:10" ht="175.5" customHeight="1">
+      <c r="B52" s="47"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="34" t="s">
         <v>448</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="34" t="s">
         <v>449</v>
       </c>
-      <c r="F52" s="40" t="s">
+      <c r="F52" s="34" t="s">
         <v>485</v>
       </c>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-    </row>
-    <row r="53" spans="2:8" ht="170.25" customHeight="1">
-      <c r="B53" s="38"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="40" t="s">
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="2:10" ht="170.25" customHeight="1">
+      <c r="B53" s="47"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="34" t="s">
         <v>450</v>
       </c>
-      <c r="E53" s="40" t="s">
+      <c r="E53" s="34" t="s">
         <v>451</v>
       </c>
-      <c r="F53" s="40" t="s">
+      <c r="F53" s="34" t="s">
         <v>484</v>
       </c>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-    </row>
-    <row r="54" spans="2:8" ht="181.5">
-      <c r="B54" s="38"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="40" t="s">
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="2:10" ht="181.5">
+      <c r="B54" s="47"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="34" t="s">
         <v>486</v>
       </c>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40" t="s">
+      <c r="E54" s="34"/>
+      <c r="F54" s="34" t="s">
         <v>487</v>
       </c>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-    </row>
-    <row r="55" spans="2:8">
-      <c r="B55" s="39"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" s="33" t="s">
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54"/>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="46"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55"/>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="45" t="s">
         <v>357</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="48" t="s">
         <v>358</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="34" t="s">
         <v>374</v>
       </c>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="38"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="40" t="s">
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56"/>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="47"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="34" t="s">
         <v>375</v>
       </c>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="38"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="39"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-    </row>
-    <row r="60" spans="2:8" ht="33">
-      <c r="B60" s="40" t="s">
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57"/>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="47"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58"/>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" s="46"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="I59"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="2:10" ht="82.5">
+      <c r="B60" s="34" t="s">
         <v>362</v>
       </c>
-      <c r="C60" s="37" t="s">
+      <c r="C60" s="33" t="s">
         <v>361</v>
       </c>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="33" t="s">
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60"/>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" s="45" t="s">
         <v>438</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C61" s="45" t="s">
         <v>478</v>
       </c>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" s="38"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="40"/>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-    </row>
-    <row r="66" spans="2:8" ht="82.5">
-      <c r="B66" s="33" t="s">
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61"/>
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62"/>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" s="47"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="34"/>
+      <c r="I63"/>
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="47"/>
+      <c r="C64" s="47"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64"/>
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="46"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="34"/>
+      <c r="I65"/>
+      <c r="J65"/>
+    </row>
+    <row r="66" spans="2:10" ht="82.5">
+      <c r="B66" s="45" t="s">
         <v>440</v>
       </c>
-      <c r="C66" s="33" t="s">
+      <c r="C66" s="45" t="s">
         <v>479</v>
       </c>
-      <c r="D66" s="40" t="s">
+      <c r="D66" s="34" t="s">
         <v>441</v>
       </c>
-      <c r="E66" s="40" t="s">
+      <c r="E66" s="34" t="s">
         <v>443</v>
       </c>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-    </row>
-    <row r="67" spans="2:8" ht="99">
-      <c r="B67" s="38"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="40" t="s">
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66"/>
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="2:10" ht="82.5">
+      <c r="B67" s="47"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="34" t="s">
         <v>442</v>
       </c>
-      <c r="E67" s="40" t="s">
+      <c r="E67" s="34" t="s">
         <v>444</v>
       </c>
-      <c r="F67" s="40"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="40"/>
-    </row>
-    <row r="68" spans="2:8" ht="66">
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="40" t="s">
+      <c r="F67" s="34"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="34"/>
+      <c r="I67"/>
+      <c r="J67"/>
+    </row>
+    <row r="68" spans="2:10" ht="49.5">
+      <c r="B68" s="47"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="34" t="s">
         <v>445</v>
       </c>
-      <c r="E68" s="40" t="s">
+      <c r="E68" s="34" t="s">
         <v>446</v>
       </c>
-      <c r="F68" s="40"/>
-      <c r="G68" s="40"/>
-      <c r="H68" s="40"/>
-    </row>
-    <row r="69" spans="2:8">
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="34"/>
+      <c r="I68"/>
+      <c r="J68"/>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="34"/>
+      <c r="I69"/>
+      <c r="J69"/>
+    </row>
+    <row r="70" spans="2:10">
+      <c r="I70"/>
+      <c r="J70"/>
+    </row>
+    <row r="71" spans="2:10">
+      <c r="I71"/>
+      <c r="J71"/>
     </row>
   </sheetData>
+  <autoFilter ref="B2:I69" xr:uid="{C388FA55-A5F7-46B9-B73C-9EEEF04696AA}"/>
   <mergeCells count="24">
+    <mergeCell ref="B48:B55"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="C33:C40"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
     <mergeCell ref="C6:C15"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="C16:C25"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="C33:C40"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="B48:B55"/>
-    <mergeCell ref="C48:C55"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B412B36A-BA8A-4C88-99A8-0A692354F987}">
+  <dimension ref="B3:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6">
+      <c r="B3" s="19" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="3">
+        <f>COUNTIF('역할 분담'!$I:$I,B5)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <f>COUNTIF('역할 분담'!$I:$I,C5)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f>COUNTIF('역할 분담'!$I:$I,D5)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <f>COUNTIF('역할 분담'!$I:$I,E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUM(B6:E6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C7" t="s">
+        <v>492</v>
+      </c>
+      <c r="D7" t="s">
+        <v>340</v>
+      </c>
+      <c r="E7" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>499</v>
+      </c>
+      <c r="C8" t="s">
+        <v>493</v>
+      </c>
+      <c r="D8" t="s">
+        <v>498</v>
+      </c>
+      <c r="E8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="C9" t="s">
+        <v>497</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>